<commit_message>
error corr, rev chap3, beg reconstruction par
</commit_message>
<xml_diff>
--- a/documents/Tableau de proposition des rapporteurs & membres du jury.xlsx
+++ b/documents/Tableau de proposition des rapporteurs & membres du jury.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14760"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="33600" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="formulaire" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="673">
   <si>
     <t>N° ED 160 - Électronique, Électrotechnique, Automatique de Lyon (EEA)</t>
   </si>
@@ -5517,6 +5517,10 @@
     <xf numFmtId="14" fontId="24" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5526,10 +5530,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -5576,8 +5576,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>4339855</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>213</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7273,8 +7273,8 @@
   </sheetPr>
   <dimension ref="A2:E278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="C211" sqref="C211"/>
+    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="C219" sqref="C219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -7666,16 +7666,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C2" s="110" t="s">
+      <c r="C2" s="108" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="110"/>
+      <c r="D2" s="108"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="C3" s="109" t="s">
+      <c r="C3" s="111" t="s">
         <v>163</v>
       </c>
-      <c r="D3" s="109"/>
+      <c r="D3" s="111"/>
     </row>
     <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
@@ -8163,7 +8163,7 @@
       <c r="B45" s="70" t="s">
         <v>489</v>
       </c>
-      <c r="C45" s="111" t="s">
+      <c r="C45" s="107" t="s">
         <v>611</v>
       </c>
       <c r="D45" s="19"/>
@@ -8175,6 +8175,9 @@
       <c r="B46" s="52" t="s">
         <v>490</v>
       </c>
+      <c r="C46" s="46" t="s">
+        <v>623</v>
+      </c>
       <c r="D46" s="19"/>
     </row>
     <row r="47" spans="1:5" s="8" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -8184,6 +8187,9 @@
       <c r="B47" s="70" t="s">
         <v>491</v>
       </c>
+      <c r="C47" s="102" t="s">
+        <v>612</v>
+      </c>
       <c r="D47" s="18"/>
     </row>
     <row r="48" spans="1:5" s="8" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -8193,9 +8199,6 @@
       <c r="B48" s="73" t="s">
         <v>494</v>
       </c>
-      <c r="C48" s="46" t="s">
-        <v>623</v>
-      </c>
       <c r="D48" s="18"/>
     </row>
     <row r="49" spans="1:5" s="8" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8204,9 +8207,6 @@
       </c>
       <c r="B49" s="74" t="s">
         <v>145</v>
-      </c>
-      <c r="C49" s="102" t="s">
-        <v>612</v>
       </c>
       <c r="D49" s="20"/>
     </row>
@@ -8307,7 +8307,7 @@
       <c r="C58" s="23" t="s">
         <v>442</v>
       </c>
-      <c r="D58" s="107" t="s">
+      <c r="D58" s="109" t="s">
         <v>546</v>
       </c>
     </row>
@@ -8316,7 +8316,7 @@
         <v>498</v>
       </c>
       <c r="C59" s="23"/>
-      <c r="D59" s="108"/>
+      <c r="D59" s="110"/>
     </row>
     <row r="60" spans="1:5" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
@@ -8501,7 +8501,7 @@
       <c r="C74" s="23" t="s">
         <v>442</v>
       </c>
-      <c r="D74" s="107" t="s">
+      <c r="D74" s="109" t="s">
         <v>547</v>
       </c>
     </row>
@@ -8510,7 +8510,7 @@
         <v>498</v>
       </c>
       <c r="C75" s="26"/>
-      <c r="D75" s="108"/>
+      <c r="D75" s="110"/>
     </row>
     <row r="76" spans="1:4" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
@@ -8685,7 +8685,7 @@
         <v>511</v>
       </c>
       <c r="C90" s="23"/>
-      <c r="D90" s="107" t="s">
+      <c r="D90" s="109" t="s">
         <v>548</v>
       </c>
     </row>
@@ -8694,7 +8694,7 @@
         <v>498</v>
       </c>
       <c r="C91" s="26"/>
-      <c r="D91" s="108"/>
+      <c r="D91" s="110"/>
     </row>
     <row r="92" spans="1:4" s="8" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
@@ -8865,7 +8865,7 @@
       <c r="C106" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="D106" s="107" t="s">
+      <c r="D106" s="109" t="s">
         <v>549</v>
       </c>
     </row>
@@ -8874,7 +8874,7 @@
         <v>498</v>
       </c>
       <c r="C107" s="23"/>
-      <c r="D107" s="108"/>
+      <c r="D107" s="110"/>
     </row>
     <row r="108" spans="1:4" s="8" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
@@ -9074,7 +9074,7 @@
       <c r="C123" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="D123" s="107" t="s">
+      <c r="D123" s="109" t="s">
         <v>550</v>
       </c>
     </row>
@@ -9083,7 +9083,7 @@
         <v>498</v>
       </c>
       <c r="C124" s="23"/>
-      <c r="D124" s="108"/>
+      <c r="D124" s="110"/>
     </row>
     <row r="125" spans="1:4" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="8" t="s">
@@ -9283,7 +9283,7 @@
       <c r="C140" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="D140" s="107" t="s">
+      <c r="D140" s="109" t="s">
         <v>551</v>
       </c>
     </row>
@@ -9292,7 +9292,7 @@
         <v>498</v>
       </c>
       <c r="C141" s="23"/>
-      <c r="D141" s="108"/>
+      <c r="D141" s="110"/>
     </row>
     <row r="142" spans="1:4" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
@@ -9492,7 +9492,7 @@
       <c r="C157" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="D157" s="107" t="s">
+      <c r="D157" s="109" t="s">
         <v>552</v>
       </c>
     </row>
@@ -9501,7 +9501,7 @@
         <v>498</v>
       </c>
       <c r="C158" s="23"/>
-      <c r="D158" s="108"/>
+      <c r="D158" s="110"/>
     </row>
     <row r="159" spans="1:4" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
@@ -9701,7 +9701,7 @@
       <c r="C174" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="D174" s="107" t="s">
+      <c r="D174" s="109" t="s">
         <v>553</v>
       </c>
     </row>
@@ -9710,7 +9710,7 @@
         <v>498</v>
       </c>
       <c r="C175" s="23"/>
-      <c r="D175" s="108"/>
+      <c r="D175" s="110"/>
     </row>
     <row r="176" spans="1:4" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="8" t="s">
@@ -9910,7 +9910,7 @@
       <c r="C191" s="23" t="s">
         <v>120</v>
       </c>
-      <c r="D191" s="107" t="s">
+      <c r="D191" s="109" t="s">
         <v>554</v>
       </c>
     </row>
@@ -9919,7 +9919,7 @@
         <v>498</v>
       </c>
       <c r="C192" s="23"/>
-      <c r="D192" s="108"/>
+      <c r="D192" s="110"/>
     </row>
     <row r="193" spans="1:4" s="8" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="8" t="s">
@@ -10074,9 +10074,7 @@
       <c r="B205" s="61" t="s">
         <v>499</v>
       </c>
-      <c r="C205" s="48" t="s">
-        <v>599</v>
-      </c>
+      <c r="C205" s="48"/>
       <c r="D205" s="72" t="s">
         <v>493</v>
       </c>
@@ -10088,9 +10086,7 @@
       <c r="B206" s="52" t="s">
         <v>495</v>
       </c>
-      <c r="C206" s="23" t="s">
-        <v>665</v>
-      </c>
+      <c r="C206" s="23"/>
       <c r="D206" s="50" t="s">
         <v>463</v>
       </c>
@@ -10102,9 +10098,7 @@
       <c r="B207" s="52" t="s">
         <v>496</v>
       </c>
-      <c r="C207" s="23" t="s">
-        <v>666</v>
-      </c>
+      <c r="C207" s="23"/>
       <c r="D207" s="50" t="s">
         <v>464</v>
       </c>
@@ -10116,10 +10110,8 @@
       <c r="B208" s="52" t="s">
         <v>535</v>
       </c>
-      <c r="C208" s="23" t="s">
-        <v>412</v>
-      </c>
-      <c r="D208" s="107" t="s">
+      <c r="C208" s="23"/>
+      <c r="D208" s="109" t="s">
         <v>555</v>
       </c>
     </row>
@@ -10128,7 +10120,7 @@
         <v>498</v>
       </c>
       <c r="C209" s="23"/>
-      <c r="D209" s="108"/>
+      <c r="D209" s="110"/>
     </row>
     <row r="210" spans="1:4" s="8" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="8" t="s">
@@ -10137,9 +10129,7 @@
       <c r="B210" s="73" t="s">
         <v>453</v>
       </c>
-      <c r="C210" s="23" t="s">
-        <v>109</v>
-      </c>
+      <c r="C210" s="23"/>
       <c r="D210" s="76" t="s">
         <v>475</v>
       </c>
@@ -10163,9 +10153,7 @@
       <c r="B212" s="52" t="s">
         <v>537</v>
       </c>
-      <c r="C212" s="49" t="s">
-        <v>667</v>
-      </c>
+      <c r="C212" s="49"/>
       <c r="D212" s="39"/>
     </row>
     <row r="213" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -10175,9 +10163,7 @@
       <c r="B213" s="52" t="s">
         <v>538</v>
       </c>
-      <c r="C213" s="23" t="s">
-        <v>668</v>
-      </c>
+      <c r="C213" s="23"/>
       <c r="D213" s="50" t="s">
         <v>505</v>
       </c>
@@ -10189,9 +10175,7 @@
       <c r="B214" s="52" t="s">
         <v>507</v>
       </c>
-      <c r="C214" s="23" t="s">
-        <v>669</v>
-      </c>
+      <c r="C214" s="23"/>
       <c r="D214" s="10" t="s">
         <v>504</v>
       </c>
@@ -10227,9 +10211,7 @@
       <c r="B217" s="52" t="s">
         <v>469</v>
       </c>
-      <c r="C217" s="23">
-        <v>38000</v>
-      </c>
+      <c r="C217" s="23"/>
       <c r="D217" s="39"/>
     </row>
     <row r="218" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -10239,9 +10221,7 @@
       <c r="B218" s="52" t="s">
         <v>470</v>
       </c>
-      <c r="C218" s="23" t="s">
-        <v>670</v>
-      </c>
+      <c r="C218" s="23"/>
       <c r="D218" s="50" t="s">
         <v>466</v>
       </c>
@@ -10253,9 +10233,7 @@
       <c r="B219" s="62" t="s">
         <v>502</v>
       </c>
-      <c r="C219" s="24" t="s">
-        <v>607</v>
-      </c>
+      <c r="C219" s="24"/>
       <c r="D219" s="69" t="s">
         <v>467</v>
       </c>
@@ -10318,7 +10296,7 @@
         <v>541</v>
       </c>
       <c r="C225" s="23"/>
-      <c r="D225" s="107" t="s">
+      <c r="D225" s="109" t="s">
         <v>556</v>
       </c>
     </row>
@@ -10327,7 +10305,7 @@
         <v>498</v>
       </c>
       <c r="C226" s="23"/>
-      <c r="D226" s="108"/>
+      <c r="D226" s="110"/>
     </row>
     <row r="227" spans="1:4" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="8" t="s">
@@ -10481,7 +10459,9 @@
       <c r="B241" s="61" t="s">
         <v>499</v>
       </c>
-      <c r="C241" s="25"/>
+      <c r="C241" s="25" t="s">
+        <v>599</v>
+      </c>
       <c r="D241" s="72" t="s">
         <v>493</v>
       </c>
@@ -10493,7 +10473,9 @@
       <c r="B242" s="52" t="s">
         <v>495</v>
       </c>
-      <c r="C242" s="23"/>
+      <c r="C242" s="23" t="s">
+        <v>665</v>
+      </c>
       <c r="D242" s="50" t="s">
         <v>463</v>
       </c>
@@ -10505,7 +10487,9 @@
       <c r="B243" s="52" t="s">
         <v>496</v>
       </c>
-      <c r="C243" s="23"/>
+      <c r="C243" s="23" t="s">
+        <v>666</v>
+      </c>
       <c r="D243" s="50" t="s">
         <v>464</v>
       </c>
@@ -10517,8 +10501,10 @@
       <c r="B244" s="78" t="s">
         <v>545</v>
       </c>
-      <c r="C244" s="23"/>
-      <c r="D244" s="107" t="s">
+      <c r="C244" s="23" t="s">
+        <v>412</v>
+      </c>
+      <c r="D244" s="109" t="s">
         <v>557</v>
       </c>
     </row>
@@ -10527,7 +10513,7 @@
         <v>498</v>
       </c>
       <c r="C245" s="23"/>
-      <c r="D245" s="108"/>
+      <c r="D245" s="110"/>
     </row>
     <row r="246" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A246" s="8" t="s">
@@ -10536,7 +10522,9 @@
       <c r="B246" s="52" t="s">
         <v>544</v>
       </c>
-      <c r="C246" s="49"/>
+      <c r="C246" s="49" t="s">
+        <v>667</v>
+      </c>
       <c r="D246" s="39"/>
     </row>
     <row r="247" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -10546,7 +10534,9 @@
       <c r="B247" s="52" t="s">
         <v>542</v>
       </c>
-      <c r="C247" s="23"/>
+      <c r="C247" s="23" t="s">
+        <v>668</v>
+      </c>
       <c r="D247" s="39"/>
     </row>
     <row r="248" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -10556,7 +10546,9 @@
       <c r="B248" s="52" t="s">
         <v>543</v>
       </c>
-      <c r="C248" s="23"/>
+      <c r="C248" s="23" t="s">
+        <v>669</v>
+      </c>
       <c r="D248" s="39"/>
     </row>
     <row r="249" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -10566,7 +10558,9 @@
       <c r="B249" s="52" t="s">
         <v>469</v>
       </c>
-      <c r="C249" s="23"/>
+      <c r="C249" s="23">
+        <v>38000</v>
+      </c>
       <c r="D249" s="39"/>
     </row>
     <row r="250" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -10576,7 +10570,9 @@
       <c r="B250" s="52" t="s">
         <v>470</v>
       </c>
-      <c r="C250" s="23"/>
+      <c r="C250" s="23" t="s">
+        <v>670</v>
+      </c>
       <c r="D250" s="50" t="s">
         <v>466</v>
       </c>
@@ -10588,7 +10584,9 @@
       <c r="B251" s="62" t="s">
         <v>502</v>
       </c>
-      <c r="C251" s="24"/>
+      <c r="C251" s="24" t="s">
+        <v>607</v>
+      </c>
       <c r="D251" s="69" t="s">
         <v>467</v>
       </c>
@@ -10651,7 +10649,7 @@
         <v>545</v>
       </c>
       <c r="C257" s="23"/>
-      <c r="D257" s="107" t="s">
+      <c r="D257" s="109" t="s">
         <v>558</v>
       </c>
     </row>
@@ -10660,7 +10658,7 @@
         <v>498</v>
       </c>
       <c r="C258" s="23"/>
-      <c r="D258" s="108"/>
+      <c r="D258" s="110"/>
     </row>
     <row r="259" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A259" s="8" t="s">
@@ -10872,6 +10870,11 @@
   <autoFilter ref="A6:A264"/>
   <dataConsolidate/>
   <mergeCells count="15">
+    <mergeCell ref="D208:D209"/>
+    <mergeCell ref="D225:D226"/>
+    <mergeCell ref="D244:D245"/>
+    <mergeCell ref="D257:D258"/>
+    <mergeCell ref="C3:D3"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="D191:D192"/>
     <mergeCell ref="D74:D75"/>
@@ -10882,11 +10885,6 @@
     <mergeCell ref="D140:D141"/>
     <mergeCell ref="D174:D175"/>
     <mergeCell ref="D157:D158"/>
-    <mergeCell ref="D208:D209"/>
-    <mergeCell ref="D225:D226"/>
-    <mergeCell ref="D244:D245"/>
-    <mergeCell ref="D257:D258"/>
-    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <dataValidations xWindow="564" yWindow="602" count="1">
     <dataValidation errorStyle="information" showInputMessage="1" showErrorMessage="1" errorTitle="ATTENTION" error="Votre saisie est différente des valeurs de la liste" sqref="C107"/>
@@ -11795,11 +11793,11 @@
         <v>+33 4 72 44 81 47</v>
       </c>
       <c r="AJ2" t="str">
-        <f>formulaire!C48</f>
+        <f>formulaire!C46</f>
         <v>LÉTANG, Jean Michel</v>
       </c>
       <c r="AK2" t="str">
-        <f>formulaire!C49</f>
+        <f>formulaire!C47</f>
         <v>jean-michel.letang@creatis.insa-lyon.fr</v>
       </c>
       <c r="AL2" t="e">
@@ -12306,41 +12304,41 @@
         <f>formulaire!C202</f>
         <v>FRANCE</v>
       </c>
-      <c r="FH2" t="str">
+      <c r="FH2">
         <f>formulaire!C205</f>
-        <v>M.</v>
-      </c>
-      <c r="FI2" t="str">
+        <v>0</v>
+      </c>
+      <c r="FI2">
         <f>formulaire!C206</f>
-        <v>DAUVERGNE</v>
-      </c>
-      <c r="FJ2" t="str">
+        <v>0</v>
+      </c>
+      <c r="FJ2">
         <f>formulaire!C207</f>
-        <v>Denis</v>
-      </c>
-      <c r="FK2" t="str">
+        <v>0</v>
+      </c>
+      <c r="FK2">
         <f>formulaire!C208</f>
-        <v>Directeur de Recherche CNRS</v>
-      </c>
-      <c r="FL2" t="str">
+        <v>0</v>
+      </c>
+      <c r="FL2">
         <f>formulaire!C210</f>
-        <v>oui</v>
+        <v>0</v>
       </c>
       <c r="FM2">
         <f>formulaire!C211</f>
         <v>0</v>
       </c>
-      <c r="FN2" t="str">
+      <c r="FN2">
         <f>formulaire!C212</f>
-        <v>denis.dauvergne@lpsc.in2p3.fr</v>
-      </c>
-      <c r="FO2" t="str">
+        <v>0</v>
+      </c>
+      <c r="FO2">
         <f>formulaire!C213</f>
-        <v>Laboratoire de Physique Corpuscolaire de Grenoble</v>
-      </c>
-      <c r="FP2" t="str">
+        <v>0</v>
+      </c>
+      <c r="FP2">
         <f>formulaire!C214</f>
-        <v>53 Avenue des Martyrs</v>
+        <v>0</v>
       </c>
       <c r="FQ2">
         <f>formulaire!C215</f>
@@ -12352,15 +12350,15 @@
       </c>
       <c r="FS2">
         <f>formulaire!C217</f>
-        <v>38000</v>
-      </c>
-      <c r="FT2" t="str">
+        <v>0</v>
+      </c>
+      <c r="FT2">
         <f>formulaire!C218</f>
-        <v>GRENOBLE</v>
-      </c>
-      <c r="FU2" t="str">
+        <v>0</v>
+      </c>
+      <c r="FU2">
         <f>formulaire!C219</f>
-        <v>FRANCE</v>
+        <v>0</v>
       </c>
       <c r="FV2">
         <f>formulaire!C222</f>
@@ -12418,45 +12416,45 @@
         <f>formulaire!C236</f>
         <v>0</v>
       </c>
-      <c r="GJ2">
+      <c r="GJ2" t="str">
         <f>formulaire!C241</f>
-        <v>0</v>
-      </c>
-      <c r="GK2">
+        <v>M.</v>
+      </c>
+      <c r="GK2" t="str">
         <f>formulaire!C242</f>
-        <v>0</v>
-      </c>
-      <c r="GL2">
+        <v>DAUVERGNE</v>
+      </c>
+      <c r="GL2" t="str">
         <f>formulaire!C243</f>
-        <v>0</v>
-      </c>
-      <c r="GM2">
+        <v>Denis</v>
+      </c>
+      <c r="GM2" t="str">
         <f>formulaire!C244</f>
-        <v>0</v>
-      </c>
-      <c r="GN2">
+        <v>Directeur de Recherche CNRS</v>
+      </c>
+      <c r="GN2" t="str">
         <f>formulaire!C246</f>
-        <v>0</v>
-      </c>
-      <c r="GO2">
+        <v>denis.dauvergne@lpsc.in2p3.fr</v>
+      </c>
+      <c r="GO2" t="str">
         <f>formulaire!C247</f>
-        <v>0</v>
-      </c>
-      <c r="GP2">
+        <v>Laboratoire de Physique Corpuscolaire de Grenoble</v>
+      </c>
+      <c r="GP2" t="str">
         <f>formulaire!C248</f>
-        <v>0</v>
+        <v>53 Avenue des Martyrs</v>
       </c>
       <c r="GQ2">
         <f>formulaire!C249</f>
-        <v>0</v>
-      </c>
-      <c r="GR2">
+        <v>38000</v>
+      </c>
+      <c r="GR2" t="str">
         <f>formulaire!C250</f>
-        <v>0</v>
-      </c>
-      <c r="GS2">
+        <v>GRENOBLE</v>
+      </c>
+      <c r="GS2" t="str">
         <f>formulaire!C251</f>
-        <v>0</v>
+        <v>FRANCE</v>
       </c>
       <c r="GT2">
         <f>formulaire!C254</f>

</xml_diff>